<commit_message>
Código e Testes - Básicos
</commit_message>
<xml_diff>
--- a/ETF_BOM.xlsx
+++ b/ETF_BOM.xlsx
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t xml:space="preserve">Material</t>
   </si>
   <si>
     <t xml:space="preserve">Quantidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETF</t>
   </si>
   <si>
     <t xml:space="preserve">JOKER</t>
@@ -353,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -372,20 +369,6 @@
       <left style="thin"/>
       <right style="thin"/>
       <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -471,7 +454,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -492,7 +475,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,39 +495,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,23 +531,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -576,7 +551,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -584,15 +567,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,13 +656,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
@@ -735,10 +710,10 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="3"/>
@@ -751,10 +726,10 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="n">
+      <c r="B4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3"/>
@@ -767,10 +742,10 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="3"/>
@@ -783,10 +758,10 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="3"/>
@@ -799,11 +774,11 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="9" t="n">
-        <v>1</v>
+      <c r="B7" s="6" t="n">
+        <v>2</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -815,11 +790,11 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="n">
-        <v>2</v>
+      <c r="B8" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -831,10 +806,10 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="3"/>
@@ -847,10 +822,10 @@
       <c r="J9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="9" t="n">
+      <c r="B10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="3"/>
@@ -863,10 +838,10 @@
       <c r="J10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="9" t="n">
+      <c r="B11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="3"/>
@@ -895,28 +870,18 @@
       <c r="J12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="11" t="n">
-        <v>1</v>
-      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="H14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -928,7 +893,6 @@
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -5843,11 +5807,7 @@
       <c r="D999" s="3"/>
       <c r="E999" s="3"/>
     </row>
-    <row r="1000" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5870,7 +5830,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -5893,298 +5853,298 @@
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="9" t="n">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="12" t="n">
         <v>42.41</v>
       </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="12" t="n">
         <v>47.68</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="12" t="n">
         <v>6.58</v>
       </c>
-      <c r="G3" s="15" t="n">
+      <c r="G3" s="13" t="n">
         <f aca="false">40/60</f>
         <v>0.6666666667</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="14" t="n">
+      <c r="H3" s="14"/>
+      <c r="I3" s="12" t="n">
         <f aca="false">C3*(D3+E3+F3+(G3*H3))</f>
         <v>96.67</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="9" t="n">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="12" t="n">
         <v>17.19</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="12" t="n">
         <v>29.22</v>
       </c>
-      <c r="F4" s="14" t="n">
+      <c r="F4" s="12" t="n">
         <v>11.46</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="14" t="n">
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="12" t="n">
         <f aca="false">C4*(D4+E4+F4+(G4*H4))</f>
         <v>57.87</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="17" t="s">
+      <c r="J4" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="K4" s="15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="9" t="n">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="14" t="n">
+      <c r="D5" s="12" t="n">
         <v>29.95</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E5" s="12" t="n">
         <v>26.17</v>
       </c>
-      <c r="F5" s="14" t="n">
+      <c r="F5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="14" t="n">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="12" t="n">
         <f aca="false">C5*(D5+E5+F5+(G5*H5))</f>
         <v>56.12</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="9" t="n">
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="12" t="n">
         <v>4.59</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="12" t="n">
         <v>8.61</v>
       </c>
-      <c r="F6" s="14" t="n">
+      <c r="F6" s="12" t="n">
         <v>3.27</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="14" t="n">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="12" t="n">
         <f aca="false">C6*(D6+E6+F6+(G6*H6))</f>
         <v>32.94</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>28</v>
+      <c r="J6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="9" t="n">
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="12" t="n">
         <v>12.06</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="12" t="n">
         <v>9.57</v>
       </c>
-      <c r="F7" s="14" t="n">
+      <c r="F7" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="14" t="n">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="12" t="n">
         <f aca="false">C7*(D7+E7+F7+(G7*H7))</f>
         <v>21.63</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>29</v>
+      <c r="J7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9" t="n">
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="12" t="n">
         <v>0.35</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="12" t="n">
         <v>0.18</v>
       </c>
-      <c r="F8" s="14" t="n">
+      <c r="F8" s="12" t="n">
         <v>0.04</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="14" t="n">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="12" t="n">
         <f aca="false">C8*(D8+E8+F8+(G8*H8))</f>
         <v>0.57</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="9" t="n">
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="12" t="n">
         <v>42</v>
       </c>
-      <c r="E9" s="14" t="n">
+      <c r="E9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="14" t="n">
+      <c r="F9" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="14" t="n">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="12" t="n">
         <f aca="false">C9*(D9+E9+F9+(G9*H9))</f>
         <v>43</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>32</v>
+      <c r="J9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="9" t="n">
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="12" t="n">
         <v>20.15</v>
       </c>
-      <c r="E10" s="14" t="n">
+      <c r="E10" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="F10" s="14" t="n">
+      <c r="F10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="14" t="n">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="12" t="n">
         <f aca="false">C10*(D10+E10+F10+(G10*H10))</f>
         <v>28.15</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="11" t="n">
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="19" t="n">
+      <c r="D11" s="17" t="n">
         <v>24.87</v>
       </c>
-      <c r="E11" s="20" t="n">
+      <c r="E11" s="18" t="n">
         <v>18.46</v>
       </c>
-      <c r="F11" s="20" t="n">
+      <c r="F11" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="14" t="n">
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="12" t="n">
         <f aca="false">C11*(D11+E11+F11+(G11*H11))</f>
         <v>43.33</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6212,7 +6172,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -6220,7 +6180,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -11187,7 +11147,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -11210,321 +11170,321 @@
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="9" t="n">
+      <c r="C3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="12" t="n">
         <v>11.57</v>
       </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="12" t="n">
         <v>16.42</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="12" t="n">
         <v>4.43</v>
       </c>
-      <c r="G3" s="22" t="n">
+      <c r="G3" s="20" t="n">
         <f aca="false">35/60</f>
         <v>0.5833333333</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="14" t="n">
+      <c r="H3" s="21"/>
+      <c r="I3" s="12" t="n">
         <f aca="false">C3*(D3+E3+F3+(G3*H3))</f>
         <v>32.42</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="12" t="n">
         <v>16.13</v>
       </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="12" t="n">
         <v>6.5</v>
       </c>
-      <c r="F4" s="14" t="n">
+      <c r="F4" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="14" t="n">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="12" t="n">
         <f aca="false">C4*(D4+E4+F4+(G4*H4))</f>
         <v>22.63</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="9" t="n">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="14" t="n">
+      <c r="D5" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="14" t="n">
+      <c r="E5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="14" t="n">
+      <c r="F5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="14" t="n">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="12" t="n">
         <f aca="false">C5*(D5+E5+F5+(G5*H5))</f>
         <v>5</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9" t="n">
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="12" t="n">
         <v>29.95</v>
       </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="12" t="n">
         <v>26.17</v>
       </c>
-      <c r="F6" s="14" t="n">
+      <c r="F6" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="14" t="n">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="12" t="n">
         <f aca="false">C6*(D6+E6+F6+(G6*H6))</f>
         <v>56.12</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="17" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="9" t="n">
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="14" t="n">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="12" t="n">
         <f aca="false">C7*(D7+E7+F7+(G7*H7))</f>
         <v>0</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>32</v>
+      <c r="J7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9" t="n">
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="12" t="n">
         <v>20.15</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="F8" s="14" t="n">
+      <c r="F8" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="14" t="n">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="12" t="n">
         <f aca="false">C8*(D8+E8+F8+(G8*H8))</f>
         <v>28.15</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="9" t="n">
+      <c r="B9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="12" t="n">
         <v>11.24</v>
       </c>
-      <c r="E9" s="14" t="n">
+      <c r="E9" s="12" t="n">
         <v>8.45</v>
       </c>
-      <c r="F9" s="14" t="n">
+      <c r="F9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="14" t="n">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="12" t="n">
         <f aca="false">C9*(D9+E9+F9+(G9*H9))</f>
         <v>19.69</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="17" t="s">
+      <c r="J9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="12" t="n">
         <v>13.48</v>
       </c>
-      <c r="E10" s="14" t="n">
+      <c r="E10" s="12" t="n">
         <v>10.02</v>
       </c>
-      <c r="F10" s="14" t="n">
+      <c r="F10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="14" t="n">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="12" t="n">
         <f aca="false">C10*(D10+E10+F10+(G10*H10))</f>
         <v>23.5</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>49</v>
+      <c r="J10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="9" t="n">
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="12" t="n">
         <v>14.92</v>
       </c>
-      <c r="E11" s="14" t="n">
+      <c r="E11" s="12" t="n">
         <v>11.37</v>
       </c>
-      <c r="F11" s="14" t="n">
+      <c r="F11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="14" t="n">
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="12" t="n">
         <f aca="false">C11*(D11+E11+F11+(G11*H11))</f>
         <v>26.29</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>49</v>
+      <c r="J11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="9" t="n">
+      <c r="B12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="14" t="n">
+      <c r="D12" s="12" t="n">
         <v>18.86</v>
       </c>
-      <c r="E12" s="14" t="n">
+      <c r="E12" s="12" t="n">
         <v>15.01</v>
       </c>
-      <c r="F12" s="14" t="n">
+      <c r="F12" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="14" t="n">
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="12" t="n">
         <f aca="false">C12*(D12+E12+F12+(G12*H12))</f>
         <v>33.87</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>49</v>
+      <c r="J12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11552,7 +11512,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -11560,7 +11520,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -16522,7 +16482,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -16546,185 +16506,185 @@
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="12" t="n">
         <v>63.59</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="12" t="n">
         <v>25.57</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="22" t="n">
+      <c r="H3" s="20" t="n">
         <f aca="false">35/60</f>
         <v>0.5833333333</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="14" t="n">
+      <c r="I3" s="21"/>
+      <c r="J3" s="12" t="n">
         <f aca="false">C3*(E3+F3+G3+(H3*I3))</f>
         <v>89.16</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="17" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="6" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="9" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="12" t="n">
         <v>43.5</v>
       </c>
-      <c r="F4" s="14" t="n">
+      <c r="F4" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="14" t="n">
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="12" t="n">
         <f aca="false">C4*(E4+F4+G4+(H4*I4))</f>
         <v>1.0875</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="14" t="n">
+      <c r="D5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="12" t="n">
         <v>2.5</v>
       </c>
-      <c r="F5" s="14" t="n">
+      <c r="F5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="14" t="n">
+      <c r="G5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="14" t="n">
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="12" t="n">
         <f aca="false">C5*(E5+F5+G5+(H5*I5))</f>
         <v>2.5</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="18"/>
+      <c r="K5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="14" t="n">
+      <c r="E6" s="12" t="n">
         <v>1.7</v>
       </c>
-      <c r="F6" s="14" t="n">
+      <c r="F6" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="14" t="n">
+      <c r="G6" s="12" t="n">
         <v>0.17</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="14" t="n">
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="12" t="n">
         <f aca="false">C6*(E6+F6+G6+(H6*I6))</f>
         <v>26.18</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="17"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="9" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="12" t="n">
         <v>299.86</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="14" t="n">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="12" t="n">
         <f aca="false">C7*(E7+F7+G7+(H7*I7))</f>
         <v>11.9944</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="18"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E8" s="3" t="n">
@@ -16751,7 +16711,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -16759,7 +16719,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -21739,7 +21699,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -21763,101 +21723,101 @@
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="14" t="n">
+      <c r="E3" s="12" t="n">
         <v>63.59</v>
       </c>
-      <c r="F3" s="14" t="n">
+      <c r="F3" s="12" t="n">
         <v>25.57</v>
       </c>
-      <c r="G3" s="14" t="n">
+      <c r="G3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="24" t="n">
+      <c r="H3" s="22" t="n">
         <f aca="false">15/60</f>
         <v>0.25</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="14" t="n">
+      <c r="I3" s="14"/>
+      <c r="J3" s="12" t="n">
         <f aca="false">C3*(E3+F3+G3+(H3*I3))</f>
         <v>89.16</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="17" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="14" t="n">
+      <c r="E4" s="12" t="n">
         <v>1.7</v>
       </c>
-      <c r="F4" s="14" t="n">
+      <c r="F4" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="14" t="n">
+      <c r="G4" s="12" t="n">
         <v>0.17</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="14" t="n">
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="12" t="n">
         <f aca="false">C4*(E4+F4+G4+(H4*I4))</f>
         <v>26.18</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="17"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E5" s="3" t="n">
@@ -21884,7 +21844,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -21892,7 +21852,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -26887,7 +26847,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
@@ -26895,58 +26855,58 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="26" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="B2" s="26" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="28" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="B3" s="26" t="n">
+        <v>127.34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="28" t="n">
-        <v>127.34</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="B4" s="26" t="n">
+        <v>109.9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="28" t="n">
-        <v>109.9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="B5" s="26" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="28" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
+      <c r="B6" s="28" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="30" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="32" t="n">
+      <c r="B7" s="30" t="n">
         <f aca="false">SUM(B2:B6)</f>
         <v>3037.24</v>
       </c>
@@ -26954,12 +26914,12 @@
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Retirada de acentuação em nome de colunas, tratamento de fim de planilha, imprimir quadro
</commit_message>
<xml_diff>
--- a/ETF_BOM.xlsx
+++ b/ETF_BOM.xlsx
@@ -659,10 +659,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
@@ -5830,7 +5830,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -11147,7 +11147,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
@@ -16482,7 +16482,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -21699,7 +21699,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -26847,7 +26847,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>

</xml_diff>